<commit_message>
completed a few more stock tests, end sunday
</commit_message>
<xml_diff>
--- a/Historical Data/ABT/ABT_financials_quarterlyinfo.xlsx
+++ b/Historical Data/ABT/ABT_financials_quarterlyinfo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleibowitz/Desktop/Github/FinancialAnalysis/Historical Data/ABT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Desktop\Github\FinancialAnalysis\Historical Data\ABT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38180" windowHeight="24660"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="38184" windowHeight="24660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="178">
   <si>
     <t>Date</t>
   </si>
@@ -555,12 +555,18 @@
   </si>
   <si>
     <t>percentage</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>sell times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,12 +636,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -649,7 +658,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,97 +723,97 @@
             <c:numRef>
               <c:f>'Sheet 1'!$A$2:$A$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>39629.0</c:v>
+                  <c:v>39629</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39721.0</c:v>
+                  <c:v>39721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39813.0</c:v>
+                  <c:v>39813</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39903.0</c:v>
+                  <c:v>39903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39994.0</c:v>
+                  <c:v>39994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40086.0</c:v>
+                  <c:v>40086</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40178.0</c:v>
+                  <c:v>40178</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40268.0</c:v>
+                  <c:v>40268</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40359.0</c:v>
+                  <c:v>40359</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40451.0</c:v>
+                  <c:v>40451</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40543.0</c:v>
+                  <c:v>40543</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40633.0</c:v>
+                  <c:v>40633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40724.0</c:v>
+                  <c:v>40724</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40816.0</c:v>
+                  <c:v>40816</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41274.0</c:v>
+                  <c:v>41274</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41547.0</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41639.0</c:v>
+                  <c:v>41639</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41729.0</c:v>
+                  <c:v>41729</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41820.0</c:v>
+                  <c:v>41820</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41912.0</c:v>
+                  <c:v>41912</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42004.0</c:v>
+                  <c:v>42004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42094.0</c:v>
+                  <c:v>42094</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42185.0</c:v>
+                  <c:v>42185</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42277.0</c:v>
+                  <c:v>42277</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42369.0</c:v>
+                  <c:v>42369</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42460.0</c:v>
+                  <c:v>42460</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42551.0</c:v>
+                  <c:v>42551</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42643.0</c:v>
+                  <c:v>42643</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42825.0</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42916.0</c:v>
+                  <c:v>42916</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -817,99 +825,104 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0870303517917583</c:v>
+                  <c:v>8.7030351791758359E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0731156651615144</c:v>
+                  <c:v>-7.3115665161514382E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.10623949942293</c:v>
+                  <c:v>-0.10623949942292966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.0138364348980329</c:v>
+                  <c:v>-1.3836434898032891E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0516581632653061</c:v>
+                  <c:v>5.1658163265306159E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0913685061653527</c:v>
+                  <c:v>9.1368506165352761E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.024263752546768</c:v>
+                  <c:v>-2.4263752546768016E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.111996962794229</c:v>
+                  <c:v>-0.11199696279422929</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.116716590085544</c:v>
+                  <c:v>0.11671659008554407</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.0828866735690553</c:v>
+                  <c:v>-8.2886673569055325E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0237945268629494</c:v>
+                  <c:v>2.3794526862949437E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0727829202017541</c:v>
+                  <c:v>7.2782920201754073E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.0281261877613075</c:v>
+                  <c:v>-2.8126187761307535E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.280797850688341</c:v>
+                  <c:v>0.28079785068834096</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0561015545248957</c:v>
+                  <c:v>5.6101554524895701E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.154866018525641</c:v>
+                  <c:v>0.1548660185256408</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.00469595592507412</c:v>
+                  <c:v>4.6959559250741162E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0620619092216</c:v>
+                  <c:v>6.2061909221599994E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0168703659232096</c:v>
+                  <c:v>1.6870365923209559E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0824717480163501</c:v>
+                  <c:v>8.2471748016350072E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0290982230119946</c:v>
+                  <c:v>2.9098223011994606E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0593567856958003</c:v>
+                  <c:v>5.9356785695800315E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.180521610410692</c:v>
+                  <c:v>-0.18052161041069226</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.116608624649214</c:v>
+                  <c:v>0.11660862464921352</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.0685815631262524</c:v>
+                  <c:v>-6.8581563126252423E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.0602438651568795</c:v>
+                  <c:v>-6.0243865156879517E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0758076805950729</c:v>
+                  <c:v>7.580768059507291E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0501300295547404</c:v>
+                  <c:v>5.0130029554740378E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0945733168205359</c:v>
+                  <c:v>9.4573316820535935E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DF47-4364-AC8D-4EC1F9E8700F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -941,97 +954,97 @@
             <c:numRef>
               <c:f>'Sheet 1'!$A$2:$A$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>39629.0</c:v>
+                  <c:v>39629</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39721.0</c:v>
+                  <c:v>39721</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39813.0</c:v>
+                  <c:v>39813</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39903.0</c:v>
+                  <c:v>39903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39994.0</c:v>
+                  <c:v>39994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40086.0</c:v>
+                  <c:v>40086</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40178.0</c:v>
+                  <c:v>40178</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40268.0</c:v>
+                  <c:v>40268</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40359.0</c:v>
+                  <c:v>40359</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40451.0</c:v>
+                  <c:v>40451</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40543.0</c:v>
+                  <c:v>40543</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40633.0</c:v>
+                  <c:v>40633</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40724.0</c:v>
+                  <c:v>40724</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40816.0</c:v>
+                  <c:v>40816</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41274.0</c:v>
+                  <c:v>41274</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41547.0</c:v>
+                  <c:v>41547</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41639.0</c:v>
+                  <c:v>41639</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41729.0</c:v>
+                  <c:v>41729</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41820.0</c:v>
+                  <c:v>41820</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41912.0</c:v>
+                  <c:v>41912</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42004.0</c:v>
+                  <c:v>42004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42094.0</c:v>
+                  <c:v>42094</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42185.0</c:v>
+                  <c:v>42185</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42277.0</c:v>
+                  <c:v>42277</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42369.0</c:v>
+                  <c:v>42369</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42460.0</c:v>
+                  <c:v>42460</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42551.0</c:v>
+                  <c:v>42551</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42643.0</c:v>
+                  <c:v>42643</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42825.0</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42916.0</c:v>
+                  <c:v>42916</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,88 +1056,88 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="1">
-                  <c:v>-0.04953</c:v>
+                  <c:v>-4.9529999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.627096</c:v>
+                  <c:v>0.62709599999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.98944</c:v>
+                  <c:v>-0.98943999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.583431</c:v>
+                  <c:v>0.58343100000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.035271</c:v>
+                  <c:v>3.5270999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.604755</c:v>
+                  <c:v>0.60475500000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.642654</c:v>
+                  <c:v>-0.64265399999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.918832</c:v>
+                  <c:v>0.91883199999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.348693</c:v>
+                  <c:v>-0.34869299999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.989419</c:v>
+                  <c:v>0.98941900000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.740941</c:v>
+                  <c:v>-0.74094099999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.563952</c:v>
+                  <c:v>0.56395200000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.097596</c:v>
+                  <c:v>9.7596000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.336051</c:v>
+                  <c:v>-4.3360510000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.062636</c:v>
+                  <c:v>1.0626359999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.105</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.194</c:v>
+                  <c:v>-0.19400000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.288</c:v>
+                  <c:v>0.28799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.009</c:v>
+                  <c:v>-8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.259</c:v>
+                  <c:v>0.25900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.203</c:v>
+                  <c:v>-0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.136</c:v>
+                  <c:v>0.13600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.044</c:v>
+                  <c:v>-4.3999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.074</c:v>
+                  <c:v>7.3999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.237</c:v>
+                  <c:v>-0.23699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.301</c:v>
+                  <c:v>0.30099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.029</c:v>
+                  <c:v>-2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.256</c:v>
+                  <c:v>0.25600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.191</c:v>
@@ -1133,6 +1146,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DF47-4364-AC8D-4EC1F9E8700F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1168,7 +1186,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1218,6 +1236,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1274,7 +1293,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2233,24 +2251,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X38" sqref="X38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="8.83203125" style="2"/>
+    <col min="8" max="8" width="8.77734375" style="2"/>
     <col min="9" max="9" width="11" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="13" width="13.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
-    <col min="21" max="21" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="12.77734375" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +2324,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>39629</v>
       </c>
@@ -2365,8 +2383,11 @@
       <c r="U2" t="s">
         <v>169</v>
       </c>
+      <c r="X2" t="s">
+        <v>176</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>39721</v>
       </c>
@@ -2438,8 +2459,16 @@
         <f>I4</f>
         <v>-7.3115665161514382E-2</v>
       </c>
+      <c r="X3" s="3">
+        <f>IF(M3&lt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Y3" s="3">
+        <f>IF(AND(M3&lt;0,I4&lt;0),1,0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>39813</v>
       </c>
@@ -2504,15 +2533,23 @@
         <v>1</v>
       </c>
       <c r="T4" s="4">
-        <f>IF(AND(M4&gt;0,I5&gt;0),1,0)</f>
+        <f t="shared" ref="T3:T30" si="5">IF(AND(M4&gt;0,I5&gt;0),1,0)</f>
         <v>0</v>
       </c>
       <c r="U4" s="4">
-        <f t="shared" ref="U4:U30" si="5">I5</f>
+        <f t="shared" ref="U4:U30" si="6">I5</f>
         <v>-0.10623949942292966</v>
       </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X30" si="7">IF(M4&lt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y30" si="8">IF(AND(M4&lt;0,I5&lt;0),1,0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>39903</v>
       </c>
@@ -2573,19 +2610,27 @@
         <v>34</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S4:S31" si="6">IF(M5&gt;0,1,0)</f>
+        <f t="shared" ref="S5:S30" si="9">IF(M5&gt;0,1,0)</f>
         <v>0</v>
       </c>
       <c r="T5">
-        <f>IF(AND(M5&gt;0,I6&gt;0),1,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.3836434898032891E-2</v>
       </c>
+      <c r="X5" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>39994</v>
       </c>
@@ -2650,15 +2695,23 @@
         <v>1</v>
       </c>
       <c r="T6" s="3">
-        <f>IF(AND(M6&gt;0,I7&gt;0),1,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1658163265306159E-2</v>
       </c>
+      <c r="X6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>40086</v>
       </c>
@@ -2719,19 +2772,27 @@
         <v>44</v>
       </c>
       <c r="S7" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T7" s="3">
-        <f>IF(AND(M7&gt;0,I8&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="3">
-        <f t="shared" si="5"/>
         <v>9.1368506165352761E-2</v>
       </c>
+      <c r="X7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>40178</v>
       </c>
@@ -2792,19 +2853,27 @@
         <v>49</v>
       </c>
       <c r="S8" s="4">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U8" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T8" s="4">
-        <f>IF(AND(M8&gt;0,I9&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="4">
-        <f t="shared" si="5"/>
         <v>-2.4263752546768016E-2</v>
       </c>
+      <c r="X8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>40268</v>
       </c>
@@ -2865,19 +2934,27 @@
         <v>54</v>
       </c>
       <c r="S9">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <f>IF(AND(M9&gt;0,I10&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="5"/>
         <v>-0.11199696279422929</v>
       </c>
+      <c r="X9" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>40359</v>
       </c>
@@ -2938,19 +3015,27 @@
         <v>59</v>
       </c>
       <c r="S10" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T10" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U10" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T10" s="3">
-        <f>IF(AND(M10&gt;0,I11&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="3">
-        <f t="shared" si="5"/>
         <v>0.11671659008554407</v>
       </c>
+      <c r="X10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>40451</v>
       </c>
@@ -3011,19 +3096,27 @@
         <v>64</v>
       </c>
       <c r="S11">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <f>IF(AND(M11&gt;0,I12&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="5"/>
         <v>-8.2886673569055325E-2</v>
       </c>
+      <c r="X11" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>40543</v>
       </c>
@@ -3084,19 +3177,27 @@
         <v>69</v>
       </c>
       <c r="S12" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T12" s="3">
-        <f>IF(AND(M12&gt;0,I13&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="3">
-        <f t="shared" si="5"/>
         <v>2.3794526862949437E-2</v>
       </c>
+      <c r="X12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>40633</v>
       </c>
@@ -3157,19 +3258,27 @@
         <v>74</v>
       </c>
       <c r="S13">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <f>IF(AND(M13&gt;0,I14&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="5"/>
         <v>7.2782920201754073E-2</v>
       </c>
+      <c r="X13" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y13" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>40724</v>
       </c>
@@ -3230,19 +3339,27 @@
         <v>79</v>
       </c>
       <c r="S14" s="4">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T14" s="4">
-        <f>IF(AND(M14&gt;0,I15&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U14" s="4">
-        <f t="shared" si="5"/>
         <v>-2.8126187761307535E-2</v>
       </c>
+      <c r="X14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>40816</v>
       </c>
@@ -3303,19 +3420,27 @@
         <v>84</v>
       </c>
       <c r="S15" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T15" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U15" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T15" s="3">
-        <f>IF(AND(M15&gt;0,I16&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U15" s="3">
-        <f t="shared" si="5"/>
         <v>0.28079785068834096</v>
       </c>
+      <c r="X15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>41274</v>
       </c>
@@ -3376,19 +3501,27 @@
         <v>89</v>
       </c>
       <c r="S16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f>IF(AND(M16&gt;0,I17&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="5"/>
         <v>5.6101554524895701E-2</v>
       </c>
+      <c r="X16" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y16" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>41547</v>
       </c>
@@ -3449,19 +3582,27 @@
         <v>94</v>
       </c>
       <c r="S17" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T17" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T17" s="3">
-        <f>IF(AND(M17&gt;0,I18&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U17" s="3">
-        <f t="shared" si="5"/>
         <v>0.1548660185256408</v>
       </c>
+      <c r="X17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>41639</v>
       </c>
@@ -3522,19 +3663,27 @@
         <v>99</v>
       </c>
       <c r="S18" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U18" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T18" s="3">
-        <f>IF(AND(M18&gt;0,I19&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U18" s="3">
-        <f t="shared" si="5"/>
         <v>4.6959559250741162E-3</v>
       </c>
+      <c r="X18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>41729</v>
       </c>
@@ -3595,19 +3744,27 @@
         <v>104</v>
       </c>
       <c r="S19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <f>IF(AND(M19&gt;0,I20&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="5"/>
         <v>6.2061909221599994E-2</v>
       </c>
+      <c r="X19" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y19" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>41820</v>
       </c>
@@ -3668,19 +3825,27 @@
         <v>109</v>
       </c>
       <c r="S20" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T20" s="3">
-        <f>IF(AND(M20&gt;0,I21&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U20" s="3">
-        <f t="shared" si="5"/>
         <v>1.6870365923209559E-2</v>
       </c>
+      <c r="X20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>41912</v>
       </c>
@@ -3741,19 +3906,27 @@
         <v>114</v>
       </c>
       <c r="S21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <f>IF(AND(M21&gt;0,I22&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="5"/>
         <v>8.2471748016350072E-2</v>
       </c>
+      <c r="X21" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42004</v>
       </c>
@@ -3814,19 +3987,27 @@
         <v>119</v>
       </c>
       <c r="S22" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T22" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U22" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T22" s="3">
-        <f>IF(AND(M22&gt;0,I23&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U22" s="3">
-        <f t="shared" si="5"/>
         <v>2.9098223011994606E-2</v>
       </c>
+      <c r="X22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42094</v>
       </c>
@@ -3887,19 +4068,27 @@
         <v>123</v>
       </c>
       <c r="S23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <f>IF(AND(M23&gt;0,I24&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="5"/>
         <v>5.9356785695800315E-2</v>
       </c>
+      <c r="X23" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y23" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42185</v>
       </c>
@@ -3960,19 +4149,27 @@
         <v>128</v>
       </c>
       <c r="S24" s="4">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T24" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T24" s="4">
-        <f>IF(AND(M24&gt;0,I25&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U24" s="4">
-        <f t="shared" si="5"/>
         <v>-0.18052161041069226</v>
       </c>
+      <c r="X24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>42277</v>
       </c>
@@ -4033,19 +4230,27 @@
         <v>133</v>
       </c>
       <c r="S25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <f>IF(AND(M25&gt;0,I26&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="5"/>
         <v>0.11660862464921352</v>
       </c>
+      <c r="X25" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y25" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>42369</v>
       </c>
@@ -4106,19 +4311,27 @@
         <v>138</v>
       </c>
       <c r="S26" s="4">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T26" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T26" s="4">
-        <f>IF(AND(M26&gt;0,I27&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="4">
-        <f t="shared" si="5"/>
         <v>-6.8581563126252423E-2</v>
       </c>
+      <c r="X26">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>42460</v>
       </c>
@@ -4179,19 +4392,27 @@
         <v>143</v>
       </c>
       <c r="S27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <f>IF(AND(M27&gt;0,I28&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="5"/>
         <v>-6.0243865156879517E-2</v>
       </c>
+      <c r="X27" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y27" s="3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>42551</v>
       </c>
@@ -4252,19 +4473,27 @@
         <v>148</v>
       </c>
       <c r="S28" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T28" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U28" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T28" s="3">
-        <f>IF(AND(M28&gt;0,I29&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U28" s="3">
-        <f t="shared" si="5"/>
         <v>7.580768059507291E-2</v>
       </c>
+      <c r="X28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>42643</v>
       </c>
@@ -4325,19 +4554,27 @@
         <v>153</v>
       </c>
       <c r="S29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <f>IF(AND(M29&gt;0,I30&gt;0),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="5"/>
         <v>5.0130029554740378E-2</v>
       </c>
+      <c r="X29" s="4">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Y29" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>42825</v>
       </c>
@@ -4398,19 +4635,27 @@
         <v>158</v>
       </c>
       <c r="S30" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T30" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="U30" s="3">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="T30" s="3">
-        <f>IF(AND(M30&gt;0,I31&gt;0),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="U30" s="3">
-        <f t="shared" si="5"/>
         <v>9.4573316820535935E-2</v>
       </c>
+      <c r="X30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>42916</v>
       </c>
@@ -4471,7 +4716,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="T32" t="s">
         <v>170</v>
       </c>
@@ -4480,7 +4725,7 @@
         <v>-0.40773261326794985</v>
       </c>
     </row>
-    <row r="33" spans="19:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="19:26" x14ac:dyDescent="0.3">
       <c r="T33" t="s">
         <v>171</v>
       </c>
@@ -4489,7 +4734,7 @@
         <v>0.94024719786902122</v>
       </c>
     </row>
-    <row r="34" spans="19:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="19:26" x14ac:dyDescent="0.3">
       <c r="T34" t="s">
         <v>172</v>
       </c>
@@ -4498,7 +4743,7 @@
         <v>0.53251458460107137</v>
       </c>
     </row>
-    <row r="37" spans="19:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="19:26" x14ac:dyDescent="0.3">
       <c r="S37" t="s">
         <v>173</v>
       </c>
@@ -4508,8 +4753,17 @@
       <c r="U37" t="s">
         <v>175</v>
       </c>
+      <c r="X37" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>175</v>
+      </c>
     </row>
-    <row r="38" spans="19:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="19:26" x14ac:dyDescent="0.3">
       <c r="S38">
         <f>SUM(S3:S30)</f>
         <v>16</v>
@@ -4521,6 +4775,18 @@
       <c r="U38">
         <f>T38/S38</f>
         <v>0.6875</v>
+      </c>
+      <c r="X38">
+        <f>SUM(X3:X30)</f>
+        <v>12</v>
+      </c>
+      <c r="Y38">
+        <f>SUM(Y3:Y30)</f>
+        <v>5</v>
+      </c>
+      <c r="Z38">
+        <f>Y38/X38</f>
+        <v>0.41666666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>